<commit_message>
16/05/2020 - BD FINAL
</commit_message>
<xml_diff>
--- a/Project_spmedgruop/Modelagem MER/Modelo_Descritivos.xlsx
+++ b/Project_spmedgruop/Modelagem MER/Modelo_Descritivos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Henrique\SENAI\2º sem\SpMedGroup\Project_spmedgruop\Modelagem MER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Henrique\SENAI\2º sem\Backand\Senai_SpMedGroup_BackEnd_BD_manha_henriquebarreirosantana\Project_spmedgruop\Modelagem MER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06BC984-15AD-4496-8650-AF9226BA0A07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3B36CC-E39A-4529-AB0C-413F02C42751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6B3045F8-3B33-4B2D-B04E-E2BDBC4F2986}"/>
+    <workbookView xWindow="2190" yWindow="0" windowWidth="15375" windowHeight="7875" xr2:uid="{6B3045F8-3B33-4B2D-B04E-E2BDBC4F2986}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>TipoUsuario</t>
   </si>
@@ -108,9 +108,6 @@
     <t>DataConsulta</t>
   </si>
   <si>
-    <t>Situação</t>
-  </si>
-  <si>
     <t>HorarioFuncionamento</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>Logradouro</t>
+  </si>
+  <si>
+    <t>IDSituação</t>
   </si>
 </sst>
 </file>
@@ -266,27 +266,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,7 +605,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,34 +621,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="18"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="1"/>
       <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="19"/>
-      <c r="L1" s="18" t="s">
+      <c r="J1" s="18"/>
+      <c r="L1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="18"/>
+      <c r="M1" s="22"/>
       <c r="N1" s="1"/>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="18"/>
+      <c r="P1" s="22"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="17" t="s">
+      <c r="R1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="17"/>
+      <c r="S1" s="21"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -731,10 +731,10 @@
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="16"/>
+      <c r="I4" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="17"/>
       <c r="L4" s="10" t="s">
         <v>18</v>
       </c>
@@ -761,10 +761,10 @@
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="16"/>
+      <c r="I5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="17"/>
       <c r="L5" s="7" t="s">
         <v>16</v>
       </c>
@@ -773,16 +773,16 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
-      <c r="R5" s="16" t="s">
+      <c r="R5" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="S5" s="16"/>
+      <c r="S5" s="17"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="2"/>
@@ -791,10 +791,10 @@
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="16"/>
+      <c r="I6" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="17"/>
       <c r="L6" s="7" t="s">
         <v>9</v>
       </c>
@@ -811,10 +811,10 @@
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="15"/>
+      <c r="C7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="16"/>
       <c r="E7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="7" t="s">
@@ -826,22 +826,22 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="7" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="S7" s="7"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="11"/>
-      <c r="C8" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="15"/>
+      <c r="C8" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="16"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="19"/>
+      <c r="F8" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="18"/>
       <c r="H8" s="2"/>
       <c r="I8" s="9" t="s">
         <v>6</v>
@@ -853,22 +853,22 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S8" s="7"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="15"/>
+      <c r="C9" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="16"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="16"/>
+      <c r="F9" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="17"/>
       <c r="H9" s="2"/>
       <c r="I9" s="9" t="s">
         <v>4</v>
@@ -880,23 +880,23 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
-      <c r="R9" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="S9" s="15"/>
+      <c r="R9" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="S9" s="16"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="15"/>
+      <c r="C10" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="16"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="16"/>
+      <c r="F10" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="17"/>
       <c r="H10" s="2"/>
       <c r="I10" s="9" t="s">
         <v>5</v>
@@ -906,26 +906,26 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
-      <c r="R10" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="S10" s="15"/>
+      <c r="R10" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="S10" s="16"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="15"/>
+      <c r="C11" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="16"/>
       <c r="E11" s="2"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="16"/>
+      <c r="I11" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="17"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
@@ -935,53 +935,54 @@
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="20"/>
+      <c r="F12" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="19"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="J12" s="22"/>
+      <c r="I12" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="20"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="P13" s="14"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C14" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C14" s="15" t="s">
+      <c r="D14" s="16"/>
+      <c r="F14" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="F14" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="16"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C15" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="15"/>
+      <c r="D15" s="16"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
       <c r="H15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K15" s="14"/>
     </row>
@@ -989,14 +990,15 @@
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
     </row>
-    <row r="17" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G17" s="13"/>
       <c r="K17" s="14"/>
+      <c r="O17" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I6:J6"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="C13:D13"/>
@@ -1005,14 +1007,17 @@
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="R10:S10"/>
     <mergeCell ref="R9:S9"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F12:G12"/>
-    <mergeCell ref="I4:J4"/>
     <mergeCell ref="R5:S5"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I6:J6"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C9:D9"/>
@@ -1020,8 +1025,7 @@
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F14:G14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>